<commit_message>
added somee attributes as suggested by UFi
</commit_message>
<xml_diff>
--- a/required/latex-lab/latex-lab-namespace.xlsx
+++ b/required/latex-lab/latex-lab-namespace.xlsx
@@ -20,11 +20,11 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1711320318" val="1068" rev="124" rev64="64" revOS="1" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1711320318" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1711320318" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1711320318"/>
-      <pm:sortOptions xmlns:pm="smNativeData" id="1711320318">
+      <pm:revision xmlns:pm="smNativeData" day="1711665724" val="1068" rev="124" rev64="64" revOS="1" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1711665724" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1711665724" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1711665724"/>
+      <pm:sortOptions xmlns:pm="smNativeData" id="1711665724">
         <pm:column colId="7"/>
         <pm:column colId="-1"/>
         <pm:column colId="-1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="214">
   <si>
     <t>Version history</t>
   </si>
@@ -104,6 +104,9 @@
     <t>Initial version (draft)</t>
   </si>
   <si>
+    <t>Added a few more attributes</t>
+  </si>
+  <si>
     <t>suggested LaTeX namespace</t>
   </si>
   <si>
@@ -656,6 +659,98 @@
     <t>/O /List /ListNumbering/Description</t>
   </si>
   <si>
+    <t>inline</t>
+  </si>
+  <si>
+    <t>/O /Layout /Placement/Inline</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>display</t>
+  </si>
+  <si>
+    <t>/O /Layout /Placement/Block</t>
+  </si>
+  <si>
+    <t>TH-col</t>
+  </si>
+  <si>
+    <t>/O /Table /Scope /Column</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>TH-row</t>
+  </si>
+  <si>
+    <t>/O /Table /Scope /Row</t>
+  </si>
+  <si>
+    <t>TH-both</t>
+  </si>
+  <si>
+    <t>/O /Table /Scope /Both</t>
+  </si>
+  <si>
+    <r>
+      <t>colspan-</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+        <family val="1"/>
+        <sz val="10"/>
+        <b val="0"/>
+        <i/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:charSpec xmlns:pm="smNativeData" id="1711665724">
+              <pm:latin face="Arial" sz="200" weight="normal" i="1"/>
+              <pm:cs/>
+              <pm:ea/>
+            </pm:charSpec>
+          </ext>
+        </extLst>
+      </rPr>
+      <t>&lt;number&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/O /Table /ColSpan </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="0"/>
+        <family val="1"/>
+        <sz val="10"/>
+        <b val="0"/>
+        <i/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:charSpec xmlns:pm="smNativeData" id="1711665724">
+              <pm:latin face="Arial" sz="200" weight="normal" i="1"/>
+              <pm:cs/>
+              <pm:ea/>
+            </pm:charSpec>
+          </ext>
+        </extLst>
+      </rPr>
+      <t>&lt;number&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>these are generated on the fly when necessary, e.g., colspan-2, colspan-7, ... They can't be predefined since any number is possible in theory.</t>
+  </si>
+  <si>
+    <t>possible values</t>
+  </si>
+  <si>
     <t xml:space="preserve">\l__tbl_cellattribute_tl </t>
   </si>
   <si>
@@ -681,6 +776,9 @@
   </si>
   <si>
     <t>\l__tag_L_attr_class_tl</t>
+  </si>
+  <si>
+    <t>set based on list type</t>
   </si>
   <si>
     <t>list, itemize, enumerate, description</t>
@@ -701,7 +799,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <family val="1"/>
@@ -709,7 +807,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1711320318" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1711665724" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -724,7 +822,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1711320318" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1711665724" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -740,7 +838,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1711320318" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1711665724" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -755,8 +853,24 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1711320318" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1711665724" ulstyle="none" kern="1">
             <pm:latin face="Courier New" sz="200" lang="default"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="1"/>
+      <i/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1711665724" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
           </pm:charSpec>
@@ -777,7 +891,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1711320318" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1711665724" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -788,7 +902,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1711320318" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1711665724" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -810,7 +924,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1711320318"/>
+          <pm:border xmlns:pm="smNativeData" id="1711665724"/>
         </ext>
       </extLst>
     </border>
@@ -829,7 +943,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1711320318"/>
+          <pm:border xmlns:pm="smNativeData" id="1711665724"/>
         </ext>
       </extLst>
     </border>
@@ -848,7 +962,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1711320318"/>
+          <pm:border xmlns:pm="smNativeData" id="1711665724"/>
         </ext>
       </extLst>
     </border>
@@ -856,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -866,9 +980,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -881,9 +992,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -912,11 +1020,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,10 +1034,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1711320318" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1711665724" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1711320318" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1711665724" count="1">
         <pm:color name="Color 24" rgb="FFFF9E"/>
       </pm:colors>
     </ext>
@@ -1192,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1206,23 +1315,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="19" t="n">
+      <c r="A3" s="17" t="n">
         <v>45375</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="19" t="n">
+        <v>45379</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1711320318" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1711665724" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1231,14 +1348,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711320318" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711665724" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1253,7 +1370,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
@@ -1270,37 +1387,37 @@
     <col min="11" max="16384" width="16.936937" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1">
-      <c r="A1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="J1" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="2:2" s="1" customFormat="1">
-      <c r="B2" s="16"/>
+      <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3"/>
@@ -1308,795 +1425,785 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="2:8">
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="6:6">
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="3:8">
       <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
         <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8">
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="3:8">
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="3:8">
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="3:8">
-      <c r="C16" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>34</v>
+      <c r="C16" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="5:8">
-      <c r="E17" s="17" t="s">
-        <v>34</v>
+      <c r="E17" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="3:8">
       <c r="C18" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8">
       <c r="C23" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>56</v>
-      </c>
-      <c r="J23"/>
-    </row>
-    <row r="24" spans="3:10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8">
       <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D24"/>
       <c r="E24" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>56</v>
-      </c>
-      <c r="J24"/>
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D26"/>
       <c r="F26" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
-      </c>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
-      </c>
-      <c r="J27"/>
+        <v>74</v>
+      </c>
     </row>
     <row r="28" spans="3:8">
       <c r="C28" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="3:8">
       <c r="C29" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D29"/>
       <c r="E29" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="3:8">
       <c r="C30" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D30"/>
       <c r="E30" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31"/>
       <c r="H31" t="s">
-        <v>91</v>
-      </c>
-      <c r="J31" s="15" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="J31" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H32" t="s">
-        <v>91</v>
-      </c>
-      <c r="J32"/>
+        <v>92</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D33"/>
       <c r="H33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H36" t="s">
-        <v>91</v>
-      </c>
-      <c r="J36"/>
-    </row>
-    <row r="37" spans="1:10">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D37"/>
       <c r="E37" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H37" t="s">
-        <v>112</v>
-      </c>
-      <c r="J37"/>
+        <v>113</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D38"/>
       <c r="E38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" t="s">
         <v>113</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D39"/>
       <c r="E39" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H39" t="s">
-        <v>112</v>
-      </c>
-      <c r="J39"/>
+        <v>113</v>
+      </c>
     </row>
     <row r="40" spans="3:10">
       <c r="C40" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D40"/>
       <c r="E40" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H40" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J40" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41"/>
       <c r="C41" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D41"/>
       <c r="E41" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H41" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J41" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="3:10">
       <c r="C42" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J42" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="3:8">
       <c r="C43" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H43" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="3:8">
       <c r="C44" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H44" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H45" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="2:10">
       <c r="B47" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J47" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="2:10">
       <c r="B48" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J48" t="s">
         <v>141</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J48" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H49" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>146</v>
+        <v>55</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H50" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H51" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2108,7 +2215,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1711320318" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1711665724" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2117,14 +2224,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711320318" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711665724" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2151,344 +2258,344 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="5:5">
-      <c r="E2" s="21"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B3" t="n">
         <v>114</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="21"/>
+      <c r="D3" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="n">
         <v>1182</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="21"/>
+      <c r="D4" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="n">
         <v>1452.14820000000009</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E5" s="21"/>
+      <c r="D5" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>1458.14879999999994</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E6" s="21"/>
+      <c r="D6" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="n">
         <v>3857</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E7" s="21"/>
+      <c r="D7" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" t="n">
         <v>196</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" s="21"/>
+      <c r="D8" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" t="n">
         <v>287</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E9" s="21"/>
+      <c r="D9" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" t="n">
         <v>517</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E10" s="21"/>
+      <c r="D10" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" t="n">
         <v>527.541000000000054</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E11" s="21"/>
+      <c r="D11" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" t="n">
         <v>2074</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="E12" s="21"/>
+      <c r="D12" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13" t="n">
         <v>2075</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E13" s="21"/>
+      <c r="D13" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B14" t="n">
         <v>361</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="E14" s="21"/>
+      <c r="D14" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B15" t="n">
         <v>162.163999999999959</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E15" s="21"/>
+      <c r="D15" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="E16" s="21"/>
+      <c r="D16" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B17" t="n">
         <v>2022</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="E17" s="21"/>
+      <c r="D17" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B18" t="n">
         <v>260</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="E18" s="21"/>
+      <c r="D18" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B19" t="n">
         <v>374</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E19" s="21"/>
+      <c r="D19" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B20" t="n">
         <v>394</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="E20" s="21"/>
+      <c r="D20" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B21" t="n">
         <v>409</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="E21" s="21"/>
+      <c r="D21" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" s="14" t="n">
+        <v>92</v>
+      </c>
+      <c r="B22" s="12" t="n">
         <v>674.706999999999994</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E22" s="21"/>
+      <c r="D22" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B23" t="n">
         <v>209</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="E23" s="21"/>
+      <c r="D23" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="14" t="n">
+        <v>129</v>
+      </c>
+      <c r="B24" s="12" t="n">
         <v>196.275000000000006</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="E24" s="21"/>
+      <c r="D24" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B25" t="n">
         <v>301</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="E25" s="21"/>
+      <c r="D25" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B26" t="n">
         <v>365</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="E26" s="21"/>
+      <c r="D26" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B27" t="n">
         <v>376</v>
       </c>
-      <c r="D27" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E27" s="21"/>
+      <c r="D27" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="4:4">
-      <c r="D28" s="13"/>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" spans="4:4">
-      <c r="D29" s="13"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="4:4">
-      <c r="D30" s="13"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="4:4">
-      <c r="D31" s="13"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="4:4">
-      <c r="D32" s="13"/>
+      <c r="D32" s="11"/>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" s="13"/>
+      <c r="D33" s="11"/>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1711320318" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1711665724" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2497,14 +2604,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711320318" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711665724" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2515,10 +2622,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -2527,146 +2634,208 @@
     <col min="2" max="2" width="28.153153" customWidth="1" style="2"/>
     <col min="3" max="3" width="29.054054" customWidth="1" style="2"/>
     <col min="4" max="6" width="15.477477" customWidth="1"/>
-    <col min="7" max="7" width="28.864865" customWidth="1" style="7"/>
+    <col min="7" max="7" width="37.990991" customWidth="1" style="3"/>
     <col min="8" max="16384" width="15.477477" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1">
-      <c r="A1" s="5" t="s">
-        <v>180</v>
+    <row r="1" spans="1:7" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="B1"/>
-      <c r="C1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>10</v>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="0" customFormat="1">
       <c r="A2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="G2" s="7"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" s="0" customFormat="1">
-      <c r="A3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
         <v>183</v>
       </c>
+      <c r="D3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="4" spans="1:7" s="0" customFormat="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" s="0" customFormat="1">
-      <c r="A5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="7"/>
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" s="0" customFormat="1">
-      <c r="A6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="7"/>
+      <c r="A6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" s="0" customFormat="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" s="0" customFormat="1">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="G8" s="7"/>
+      <c r="C8" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="E8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" s="0" customFormat="1">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="G9" s="7"/>
+      <c r="C9" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" s="0" customFormat="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" s="0" customFormat="1">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="G11" s="7"/>
+      <c r="C11" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" s="0" customFormat="1">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>195</v>
+      </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" s="0" customFormat="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="G13" s="7"/>
+      <c r="C12" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14"/>
+      <c r="A14" s="20" t="s">
+        <v>199</v>
+      </c>
       <c r="B14"/>
-      <c r="C14"/>
-      <c r="G14"/>
+      <c r="C14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15"/>
@@ -2710,17 +2879,11 @@
       <c r="C21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="G22"/>
-    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1711320318" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1711665724" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2729,14 +2892,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711320318" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711665724" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2747,128 +2910,143 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="1" max="1" width="26.837838" customWidth="1"/>
     <col min="2" max="2" width="8.918919" customWidth="1"/>
-    <col min="3" max="3" width="29.054054" customWidth="1"/>
-    <col min="4" max="4" width="9.324324" customWidth="1"/>
-    <col min="5" max="5" width="18.432432" customWidth="1" style="22"/>
+    <col min="3" max="4" width="29.054054" customWidth="1"/>
+    <col min="5" max="5" width="9.324324" customWidth="1"/>
+    <col min="6" max="6" width="18.432432" customWidth="1" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="D1" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="D2" s="2"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7">
+        <v>205</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7">
+        <v>205</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
+        <v>205</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7">
+        <v>205</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>195</v>
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>212</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7">
+        <v>213</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="D8" s="2"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="G9" s="7"/>
+      <c r="D9" s="2"/>
+      <c r="H9" s="6"/>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1711320318" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1711665724" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2877,14 +3055,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1711320318" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1711665724" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711320318" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1711665724" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>